<commit_message>
feature multithread for saving data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/user_excel_import/normal _development.xlsx
+++ b/src/test/resources/testdata/user_excel_import/normal _development.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>password</t>
   </si>
@@ -69,6 +69,39 @@
   </si>
   <si>
     <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test4@gmail.com</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test6@gmail.com</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test7@gmail.com</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test5@gmail.com</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>USER, USER</t>
   </si>
 </sst>
 </file>
@@ -406,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,6 +496,12 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -487,10 +526,93 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -498,8 +620,12 @@
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D6" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>